<commit_message>
iniciando a página inicial
</commit_message>
<xml_diff>
--- a/server/DataBase.xlsx
+++ b/server/DataBase.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marci\OneDrive\Pós PUC\Desenvolvimento Web\petshop\server\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{D1512C9A-4042-4FCD-B5EB-281CE015B4D7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{0A9B57E3-D974-48ED-837D-22CB56B4A5AC}"/>
+  <xr:revisionPtr revIDLastSave="34" documentId="13_ncr:1_{D1512C9A-4042-4FCD-B5EB-281CE015B4D7}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{CBA54314-4DBF-4D4B-B269-FD7A4EA179E9}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5955" xr2:uid="{E972D0C0-4EC2-442B-83FF-87D5539D8F35}"/>
   </bookViews>
   <sheets>
-    <sheet name="Candidatos" sheetId="1" r:id="rId1"/>
+    <sheet name="Produtos" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179021"/>
   <extLst>
@@ -498,7 +498,7 @@
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>